<commit_message>
Restructured the code to use work with dataframes and avoid saving images in drive
</commit_message>
<xml_diff>
--- a/output/final.xlsx
+++ b/output/final.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -5139,38 +5127,45 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Trademark Number (210)</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Application Filing Date (220)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Class of registration (511)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Proprietor/Owner (730)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Representative/Applicant (740)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Image/Mark</t>
         </is>
       </c>
     </row>
-    <row r="2"/>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -5197,6 +5192,7 @@
           <t>Hamilton Harrison &amp; Mathews Advocates of P. O. Box 30333 - 00100, NAIROBI, Kenya</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -5224,6 +5220,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -5251,6 +5248,7 @@
           <t>Simba &amp; Simba Advocates of P. O. Box 10312 - 00100 , NAIROBI, Kenya</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -5278,6 +5276,7 @@
           <t>SIMBA &amp; SIMBA ADVOCATES  of P.O. Box 10312  – 00100,  NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5305,6 +5304,7 @@
           <t>NDUNGU NJOROGE &amp; KWACH ADVOCATES of P.O. Box 41546 - 00100,  NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5364,6 +5364,7 @@
           <t>TRIPLE LAW ADVOCATES  of P.O. BOX 49403 - 00100 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -5391,6 +5392,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -5514,6 +5516,7 @@
           <t>J. K. MUCHAE &amp; COMPANY ADVOCATES  of P.O. Box 60664 – 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -5541,6 +5544,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -5600,6 +5604,7 @@
           <t>Muiruri &amp; Wachira Advocates of P. O. Box 2119 - 00606, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -5659,6 +5664,7 @@
           <t>SIMBA &amp; SIMBA CO. Advoca tesof P. O. BOX 10312 - 00100 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -5686,6 +5692,7 @@
           <t>GICHACHI &amp; COMPANY ADVOCATES ,P.O.BOX 79659 - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -5713,6 +5720,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -5740,6 +5748,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -5747,6 +5756,7 @@
           <t>117782</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>17(Plastic strap band for packaging)</t>
@@ -5794,6 +5804,7 @@
           <t>WANAM SALE ADVOCATES &amp; PATENT ATTORNEYS , of P.O. Box 43123 - 00100 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -5821,6 +5832,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -6020,6 +6032,7 @@
           <t>119132</t>
         </is>
       </c>
+      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
           <t>9(Scientific, nautical, surveying, photographic, cinematographic, optical, weighing, measuring, signaling, checking (supervision), life -saving and teaching apparatus and instruments; apparatus and instruments for conducting, switching , transforming, accumulating, regulating or controlling electricity; apparatus for recording, transmission or reproduction of sound or images; magnetic data carriers, recording discs; compact discs, DVDs and other digital recording media; mechanisms for co in-operated apparatus; cash registers, calculating machines, data processing equipment, computers; computer software; fire -extinguishing I". apparatus. ) and 11(Apparatus for lighting, heating, steam generating, cooking, refrigerating, drying, ventilating, water supply and sanitary purposes )</t>
@@ -6035,6 +6048,7 @@
           <t>GICHACHI &amp; COMP ANY ADVOCATES of P. O. BOX 79659  - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -6062,6 +6076,7 @@
           <t>Iseme Kamau &amp; Maema Advocates of P.O. Box 11866 - 00400 , NAIROBI, Kenya</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -6121,6 +6136,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -6180,6 +6196,7 @@
           <t>KAPLAN &amp; STRATTON ADVOCATES of P. O. BOX 40111 – 00100 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -6207,6 +6224,7 @@
           <t>CFL Advocates  of P.O. Box 23555 - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -6234,6 +6252,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -6256,6 +6275,8 @@
           <t>Lincoln Global, Inc  of 9160 Norwalk Boulevard, Santa Fe Springs, California 90670, United States of America</t>
         </is>
       </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -6283,6 +6304,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -6433,6 +6455,8 @@
           <t>De Ruiter Intellectual Property B.V.  of NEERLANDENWEG 55 1181 ZR AMSTEL VEEN , Netherlands</t>
         </is>
       </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6460,6 +6484,7 @@
           <t>J. K. MUCHAE &amp; COMPANY A DVOCATES  of P. O. Box 60664 - 00200 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6487,6 +6512,7 @@
           <t>J.K. MUCHAE &amp; CO ADVOCAT ES of P. O. Box 60664 - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -6546,6 +6572,7 @@
           <t>Messrs Iseme Kamau &amp; Maema Advocates  of P.O. BOX 11866 - 00400, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -6573,6 +6600,7 @@
           <t>Messrs Iseme Kamau &amp; Maema Advo cates  of P.O. BOX 11866 - 00400, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -6696,6 +6724,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -6755,6 +6784,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -6782,6 +6812,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -6809,6 +6840,7 @@
           <t>CFL ADVOCATES  of P.O. Box 23555 - 00100, NAIROBI , Keny a</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -6836,6 +6868,7 @@
           <t>OWAGA AND ASSOCIATES LLP ADVOCATES  of P.O. BOX 14826 - 00100, Nairobi , Kenya</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -6863,6 +6896,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -6890,6 +6924,7 @@
           <t>J. K.   &amp; COMPANY ADVOCATES of P.O. Box 60664 -00200, Nairobi , Kenya</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6912,13 +6947,20 @@
           <t>JARAMOGI OGINGA ODINGA UNIVERSITY</t>
         </is>
       </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
     </row>
     <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -6931,6 +6973,7 @@
           <t>16/02/2023</t>
         </is>
       </c>
+      <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
           <t>KENYA MORTGAGE REFINANCE COMPANY PLC  of P.O. BOX 15494 - 00100, NAIROBI, Kenya</t>
@@ -6941,6 +6984,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -6968,6 +7012,7 @@
           <t>Kieti Advocates LLP  of P. O. Box 22602 - 00505, Nairobi , Kenya</t>
         </is>
       </c>
+      <c r="F66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -6995,6 +7040,7 @@
           <t>CFL ADVOCATES  of P.O. Box 23555 - 00100, , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -7118,6 +7164,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -7209,6 +7256,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -7236,6 +7284,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -7295,6 +7344,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -7322,6 +7372,7 @@
           <t>NJUGUNA KAMAU OKOTH ADVOCAT ES of P.O. BOX 36463 - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -7349,6 +7400,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -7457,6 +7509,7 @@
           <t>18/04/2023</t>
         </is>
       </c>
+      <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr">
         <is>
           <t>SAFE HAVEN LIMITED  of P. O. Box 66831 -00800, No.728, Maji Mazuri Road, Lavington, Nairobi, Kenya</t>
@@ -7467,6 +7520,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -7494,6 +7548,7 @@
           <t>CFL AD VOCATES  of P. O. Box 23555 -00100 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -7553,6 +7608,7 @@
           <t>Messrs J K Muchae &amp; Company Advocates  of P.O. Box 60664 - 00200,  NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -7560,6 +7616,7 @@
           <t>127460</t>
         </is>
       </c>
+      <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
           <t>7(Sewing Machines, Stitching Machines, Hemming Machines, Pedal drives for sewing machines, Whip stitch machine, Lock button machine, prize Machine, cutting cloth machine, industry sartorius, Machines for textile industry .)</t>
@@ -7575,6 +7632,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -7602,6 +7660,7 @@
           <t>CK KIOKO &amp; COMPANY ADVOCATES  of P.O. Box 2346 -00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -7725,6 +7784,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -7752,6 +7812,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -7779,6 +7840,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -7806,6 +7868,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -7833,6 +7896,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -7860,6 +7924,7 @@
           <t>WJ Itho ndeka &amp; Company Advocates Commissioners for Oaths  of P.O. BOX 53974 - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -7887,6 +7952,7 @@
           <t>WJ Ithondeka &amp; Company Advocates Commissioners for Oaths  of P.O. BOX 53974 - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -7914,6 +7980,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -7973,6 +8040,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -8096,6 +8164,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -8187,6 +8256,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -8214,6 +8284,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -8285,6 +8356,7 @@
           <t>128496</t>
         </is>
       </c>
+      <c r="B112" t="inlineStr"/>
       <c r="C112" t="inlineStr">
         <is>
           <t>5(Pharmaceutical products and substances for productive health)</t>
@@ -8396,6 +8468,7 @@
           <t>CFL ADVOCATES  of P.O. Box 23555 -00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -8423,6 +8496,7 @@
           <t>DENNIS ONYANGO &amp; ASSOCIATES  of P. O. Box 30588 -00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -8450,6 +8524,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -8477,6 +8552,7 @@
           <t>Ndungu Njoroge &amp; Kwach Advocates of P. O. Box 41546 - 00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -8499,13 +8575,20 @@
           <t>JUDY WANJIKU KIHUMBA  of P. O. Box</t>
         </is>
       </c>
+      <c r="E119" t="inlineStr"/>
+      <c r="F119" t="inlineStr"/>
     </row>
     <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
+      <c r="F120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -8533,6 +8616,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -8550,11 +8634,13 @@
           <t>7(Water pumps, generators, agricultural machines, household machinery(vacuum cleaners, hemming machines, incubators, ironing machines, juice extractors), electrical motors, construction machines. ), 8(Hardware items(cutting discs, lifting jacks hand operated, hand tools, milling cutters hand oper ated) ), 9(Safety footwear for protection against accident ) and 35(Advertising; business management)</t>
         </is>
       </c>
+      <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
+      <c r="F122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -8646,6 +8732,7 @@
           <t>DOMINIC B. OSORO ADVOCAT E &amp; COMMISSIONER FOR OATHS  of P.O. BOX 207-00606, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -8673,6 +8760,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -8700,6 +8788,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -8727,6 +8816,7 @@
           <t>J.K MUCHAE &amp; COMPANY ADVOCATES  of P. O. Box 60664 - 00200 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -8786,6 +8876,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -8813,6 +8904,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -8840,6 +8932,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -8867,6 +8960,7 @@
           <t>Talal Abu -Ghazaleh Intellectual Property  of P.O. BOX 2537 -00606, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -8894,6 +8988,7 @@
           <t>Talal Abu -Ghazaleh Intellectual Property  of P.O. BOX 2537 -00606, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -8921,6 +9016,7 @@
           <t>GICHACHI &amp; COMPANY ADVOCATES  of P.O.BOX 79659 - 00200, Agip House - First Floor, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -8948,6 +9044,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -8975,6 +9072,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -8987,6 +9085,7 @@
           <t>27/07/2023</t>
         </is>
       </c>
+      <c r="C138" t="inlineStr"/>
       <c r="D138" t="inlineStr">
         <is>
           <t>ACADIAN SEAPLANTS LIMITED  of 30 BROWN AVENUE, DARTMOUTH NOVA SCOTIA, B3B 1X8, Canada</t>
@@ -9029,6 +9128,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -9088,6 +9188,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -9115,6 +9216,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -9142,6 +9244,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -9169,6 +9272,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -9196,6 +9300,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -9223,6 +9328,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -9250,6 +9356,7 @@
           <t>J. K. MUCHAE &amp; COMPANY ADVOCATES of P.O. BOX 60664 - 00200, NAIROBI, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -9277,6 +9384,7 @@
           <t>J. K. MUCHAE &amp; COMPANY ADVOCATES  of P .O. BOX 60664 -00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -9304,6 +9412,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -9331,6 +9440,7 @@
           <t>MYIP LEGAL STUDIO  of P.O. Box 5047-00100,  NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -9385,6 +9495,8 @@
           <t>M-KOPA KENYA LIMITED  of P.O. Box 51866 - 00100,  Nairobi, Kenya</t>
         </is>
       </c>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -9444,6 +9556,7 @@
           <t>Gathiga Muhindi Advocates  of P. O. Box 855 -00618, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -9471,6 +9584,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -9562,6 +9676,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -9589,6 +9704,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -9611,6 +9727,8 @@
           <t>PROPACK (KENYA) LIMITED  of P. O. Box 48185 -00100, 740): MW &amp; Company Advocates LLP  of P.O.BOX 44468 -00100 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="E160" t="inlineStr"/>
+      <c r="F160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -9702,6 +9820,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -9729,6 +9848,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -9756,6 +9876,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -9783,6 +9904,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -9810,6 +9932,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -9837,6 +9960,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -9864,6 +9988,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -9891,6 +10016,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -9950,6 +10076,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -9977,6 +10104,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -10004,6 +10132,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -10031,6 +10160,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -10058,6 +10188,7 @@
           <t>IGERIA AND NGUGU ADVOCATES  of P.O. BOX 60635 - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -10085,6 +10216,7 @@
           <t>MURI MWANIKI  THIGE &amp; KAGENI LLP ADVOCATES  of P.O. BOX 13726 - 00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -10144,6 +10276,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -10171,6 +10304,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -10198,6 +10332,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -10242,6 +10377,7 @@
           <t>11/09/2023</t>
         </is>
       </c>
+      <c r="C183" t="inlineStr"/>
       <c r="D183" t="inlineStr">
         <is>
           <t>LONDON DISTILLERS (K) LTD  Manufacturers of alcoholic beverages  of P.O. BOX 57387 - 00200, NAIROBI, K enya</t>
@@ -10284,6 +10420,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -10311,6 +10448,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -10370,6 +10508,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -10397,6 +10536,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -10456,6 +10596,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -10547,6 +10688,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -10574,6 +10716,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -10601,6 +10744,7 @@
           <t>BOWMANS  of P. O. Box 10643 - 00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -10628,6 +10772,7 @@
           <t>BOWMANS  of P.O. Box 10643 -00100,  Nairobi</t>
         </is>
       </c>
+      <c r="F196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -10655,6 +10800,7 @@
           <t>BOWMANS  of P. O. Box 10643 - 00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -10682,6 +10828,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -10709,6 +10856,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -10736,6 +10884,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -10763,6 +10912,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -10790,6 +10940,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -10881,6 +11032,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -10908,6 +11060,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -10935,6 +11088,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -10962,6 +11116,7 @@
           <t>Kimani &amp; Muchiri Advocates LLP ,, Ambassador Court, Suite E4 Milimani Road, Nairobi</t>
         </is>
       </c>
+      <c r="F208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -10989,6 +11144,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -11016,6 +11172,7 @@
           <t>OTIENO OGOLA &amp; CO. ADVOCA TESof P.O. BOX 22671 -00100 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -11055,6 +11212,7 @@
           <t>130096</t>
         </is>
       </c>
+      <c r="B212" t="inlineStr"/>
       <c r="C212" t="inlineStr">
         <is>
           <t>5(Pharmaceuticals)</t>
@@ -11188,11 +11346,13 @@
           <t>38(Telecommunicatio ns), 39(Transport; packaging and storage of goods; travel arrangement.) and 42(Scientific and technological services and research and design relating thereto; industrial analysis and research services; design and development of computer hardware and softwa re.)</t>
         </is>
       </c>
+      <c r="D216" t="inlineStr"/>
       <c r="E216" t="inlineStr">
         <is>
           <t>OJ ADVOCATES LLP  of P. O.  Box 76683 - 00508, Nairobi</t>
         </is>
       </c>
+      <c r="F216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -11220,6 +11380,7 @@
           <t>OJ ADVOCATES LLP  of P. O. Box 76683 - 00508, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -11247,6 +11408,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -11274,6 +11436,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -11301,6 +11464,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -11328,6 +11492,7 @@
           <t>KAMAU K'ANJEJO &amp; KIRIGHA CO. ADVOCATES  of P. O. Box 10957 -00400, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -11419,6 +11584,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -11446,6 +11612,7 @@
           <t>LEE MUTUNGA LEE, KWESIGA &amp; KIPRONO ADVOCATES LLP  of P. O. Box 19200 - 00501, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -11473,6 +11640,7 @@
           <t>LEE MUTUNGA LEE, KWESIGA &amp; KIPRONO ADVOCATES LLP  of P. O. Box 19200 - 00501, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -11500,6 +11668,7 @@
           <t>LEE MUTUNGA LEE, KWESIGA &amp; KIPRONO ADVOCATES LLP  of P. O. Box 19200 -00501, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -11527,6 +11696,7 @@
           <t>LEE MUTUNGA LE E, KWESIGA &amp; KIPRONO ADVOCATES LLP  of P. O. Box 19200 - 00501, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -11554,6 +11724,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -11581,6 +11752,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -11608,6 +11780,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -11635,6 +11808,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -11834,6 +12008,7 @@
           <t>130183</t>
         </is>
       </c>
+      <c r="B239" t="inlineStr"/>
       <c r="C239" t="inlineStr">
         <is>
           <t>5(Pharmaceutical Preparations)</t>
@@ -11977,6 +12152,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -12004,6 +12180,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -12026,6 +12203,8 @@
           <t>BABA AGRO AFRICA LIMITED  of P. O. Box 16526 -80100, Mombasa, Kenya</t>
         </is>
       </c>
+      <c r="E245" t="inlineStr"/>
+      <c r="F245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -12053,6 +12232,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -12080,6 +12260,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -12107,6 +12288,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -12166,6 +12348,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -12193,6 +12376,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -12220,6 +12404,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -12247,6 +12432,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -12274,6 +12460,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -12333,6 +12520,7 @@
           <t>Talal Abu -Ghazaleh Intellectual Property Limited  of P.O. Box 2537 -00606 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -12360,6 +12548,7 @@
           <t>Talal Abu -Ghazaleh Intellectual Property Limited , of P.O. Box 2537 - 00606 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -12387,6 +12576,7 @@
           <t>Talal Abu -Ghazaleh Intellectual Property Limited , of P.O. Box 2537 -00606 , NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -12414,6 +12604,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -12441,6 +12632,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -12468,6 +12660,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -12495,6 +12688,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -12522,6 +12716,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -12549,6 +12744,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -12576,6 +12772,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -12583,6 +12780,7 @@
           <t>130292</t>
         </is>
       </c>
+      <c r="B266" t="inlineStr"/>
       <c r="C266" t="inlineStr">
         <is>
           <t>41(Golf accessories &amp; Trainings)</t>
@@ -12598,6 +12796,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -12625,6 +12824,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -12652,6 +12852,7 @@
           <t>Wawira Gachoki &amp; Partners Advocates  of P.O.Box 13796 - 00800, D elta Corner Towers, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -12743,6 +12944,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -12765,6 +12967,8 @@
           <t>HAY FESTIVAL KENYA  of P. O. Box 4327 - 30100, Kenya</t>
         </is>
       </c>
+      <c r="E272" t="inlineStr"/>
+      <c r="F272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -12792,6 +12996,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -12819,6 +13024,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -12846,6 +13052,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -12873,6 +13080,7 @@
           <t>Fredrick Omukubi Otswong'o  &amp; IP Associates  of P.O. Box 54708 - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -12900,6 +13108,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -12927,6 +13136,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -12954,6 +13164,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -12981,6 +13192,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -13040,6 +13252,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -13131,6 +13344,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -13158,6 +13372,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -13217,6 +13432,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -13276,6 +13492,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -13303,6 +13520,7 @@
           <t>KAPLAN &amp; STRATTON ADVOCATES ,P. O. BOX 40111 - 00100, Williamson House, 4th Ngong Avenue , NAIROBI , Ken ya</t>
         </is>
       </c>
+      <c r="F291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -13362,6 +13580,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -13389,6 +13608,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -13416,6 +13636,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -13443,6 +13664,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -13470,6 +13692,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -13497,6 +13720,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -13524,6 +13748,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -13551,6 +13776,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -13578,6 +13804,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -13600,6 +13827,8 @@
           <t>PEAK PERFORMANCE INTERNATIONAL  of Laikipia Road, River Gardens, Kileleshwa, P. O. Box 12767 - 00400,  Nairobi, Kenya</t>
         </is>
       </c>
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -13627,6 +13856,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -13654,6 +13884,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -13681,6 +13912,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -13740,6 +13972,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -13767,6 +14000,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -13794,6 +14028,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -13821,6 +14056,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F310" t="inlineStr"/>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -13848,6 +14084,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -13875,6 +14112,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -13902,6 +14140,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -13929,6 +14168,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F314" t="inlineStr"/>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -14010,6 +14250,7 @@
           <t>5(Pharmaceutical and veterinary preparations; sanitary preparations for medical purposes; dietetic substances adapted for medical use, food for babies; plasters, materials for dressings; material for stopping teeth, dental wax; disinfectants, sanitizers)</t>
         </is>
       </c>
+      <c r="D317" t="inlineStr"/>
       <c r="E317" t="inlineStr">
         <is>
           <t>None</t>
@@ -14111,6 +14352,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -14138,6 +14380,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -14165,6 +14408,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -14224,6 +14468,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F324" t="inlineStr"/>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -14315,6 +14560,7 @@
           <t>Krhoda &amp; Macharia Advocates of P. O. Box 56745 - 00200, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F327" t="inlineStr"/>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -14406,6 +14652,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F330" t="inlineStr"/>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -14433,6 +14680,7 @@
           <t>IGERIA &amp; Co. ADVOCATES of P.O. Box  60635 -00200, Nairobi</t>
         </is>
       </c>
+      <c r="F331" t="inlineStr"/>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -14460,6 +14708,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F332" t="inlineStr"/>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -14487,6 +14736,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F333" t="inlineStr"/>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -14642,6 +14892,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F338" t="inlineStr"/>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -14669,6 +14920,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F339" t="inlineStr"/>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -14728,6 +14980,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F341" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -14755,6 +15008,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F342" t="inlineStr"/>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -14782,6 +15036,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F343" t="inlineStr"/>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -14809,6 +15064,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F344" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -14816,6 +15072,7 @@
           <t>130610</t>
         </is>
       </c>
+      <c r="B345" t="inlineStr"/>
       <c r="C345" t="inlineStr">
         <is>
           <t>30(Spices) and 43(Restaurant)</t>
@@ -14831,6 +15088,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F345" t="inlineStr"/>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -14954,6 +15212,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F349" t="inlineStr"/>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -14981,6 +15240,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F350" t="inlineStr"/>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -15008,6 +15268,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F351" t="inlineStr"/>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -15131,6 +15392,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F355" t="inlineStr"/>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -15158,6 +15420,7 @@
           <t>Sonal Raval Advocate  of P .O. BOX 10652 - 00400, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F356" t="inlineStr"/>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -15185,6 +15448,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F357" t="inlineStr"/>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -15549,6 +15813,7 @@
           <t>30/10/2023</t>
         </is>
       </c>
+      <c r="C369" t="inlineStr"/>
       <c r="D369" t="inlineStr">
         <is>
           <t>LASA AFRICA PTY LTD  of P. O. Box 18945 -00100, Nairobi, Kenya</t>
@@ -15559,6 +15824,7 @@
           <t>MAJURA &amp; AMUNGA ADVOCATES  of P. O Box 18945 -00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F369" t="inlineStr"/>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -15586,6 +15852,7 @@
           <t>MAJURA &amp; AMUNGA ADVOCATES  of P. O Box 18945 -00100, NA IROBI , Kenya</t>
         </is>
       </c>
+      <c r="F370" t="inlineStr"/>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -15613,6 +15880,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F371" t="inlineStr"/>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -15640,6 +15908,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F372" t="inlineStr"/>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -15667,6 +15936,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F373" t="inlineStr"/>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -15694,6 +15964,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F374" t="inlineStr"/>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -15721,6 +15992,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F375" t="inlineStr"/>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -15748,6 +16020,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F376" t="inlineStr"/>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -15775,6 +16048,7 @@
           <t>MYIP LEGAL STUDIO  of P.O. Box 50474 -00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F377" t="inlineStr"/>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -15834,6 +16108,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F379" t="inlineStr"/>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -15861,6 +16136,7 @@
           <t>TRIPLEOKLAW LLP  ADVOCATES of P. O. BOX 43170 - 00100, NAIROBI , Kenya</t>
         </is>
       </c>
+      <c r="F380" t="inlineStr"/>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -16016,6 +16292,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F385" t="inlineStr"/>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -16043,6 +16320,7 @@
           <t>None</t>
         </is>
       </c>
+      <c r="F386" t="inlineStr"/>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">

</xml_diff>